<commit_message>
Improve: Copy Module hint
</commit_message>
<xml_diff>
--- a/Data/ConfigTemplate_Public.xlsx
+++ b/Data/ConfigTemplate_Public.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scep\Documents\UiPath\zid-moodle-feedbacker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13017AE-E582-4A0C-BD1D-96EF822EC60C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B88F0B3-0411-4E9E-80F8-28995F373C43}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>a@b.ch</t>
+  </si>
+  <si>
+    <t>MailTemplatePathCopyModule</t>
+  </si>
+  <si>
+    <t>Data\Input\MailTemplateCopyModule</t>
   </si>
 </sst>
 </file>
@@ -675,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z986"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -899,38 +905,48 @@
     </row>
     <row r="18" spans="1:3" ht="30">
       <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30">
+      <c r="A19" t="s">
         <v>81</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>4</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
         <v>86</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1896,6 +1912,7 @@
     <row r="984" ht="14.25" customHeight="1"/>
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
+    <row r="987" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>